<commit_message>
Recreated models for chi2 and xgboost based models, added their results to Feature Selection Method Comparisons.xlsx. Redid Test C to find the performance of a Location information only model.
</commit_message>
<xml_diff>
--- a/Jeremy Thesis/XGBoost Feature Importance Scores.xlsx
+++ b/Jeremy Thesis/XGBoost Feature Importance Scores.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\SCAL_USIgnite-911\Jeremy Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DE0BE0-2C95-41A5-AEE8-1120352BDEFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CB0BEB-4CC8-4D24-9D1C-FCB4CFF2406B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21840" yWindow="2625" windowWidth="13770" windowHeight="14160" xr2:uid="{18175824-6174-4650-8E46-74AD3EF26151}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18175824-6174-4650-8E46-74AD3EF26151}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Longitude</t>
   </si>
@@ -574,7 +573,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,248 +889,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9807A73-408B-4131-9B2F-C3EBA5D712B5}">
-  <dimension ref="A1:B28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0.18622373</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <v>0.12677258</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0.12059394</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0.10362833</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>8.0988589999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>8.0088670000000001E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8">
-        <v>5.647713E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9">
-        <v>5.2327520000000002E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>4.8520550000000003E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11">
-        <v>2.6842250000000002E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>1.6549069999999999E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>1.587384E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>1.400651E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15">
-        <v>1.347454E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16">
-        <v>1.2900460000000001E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <v>1.148917E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18">
-        <v>9.4232599999999993E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>7.3885599999999997E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20">
-        <v>5.1918800000000003E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21">
-        <v>4.4130799999999998E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22">
-        <v>4.1363499999999996E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23">
-        <v>2.68995E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>